<commit_message>
fixing bugs in csp
</commit_message>
<xml_diff>
--- a/case_input_base_190702.xlsx
+++ b/case_input_base_190702.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A880FC7-6A75-43D8-9977-084C0A62747F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283F923D-281B-4CAD-AAC5-11C9650934BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-21405" windowWidth="35910" windowHeight="19050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EIAbase" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="174">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -522,9 +522,6 @@
     <t>EIAtest</t>
   </si>
   <si>
-    <t>EIAtestCSP</t>
-  </si>
-  <si>
     <t>DECAY_RATE_PGP_STORAGE</t>
   </si>
   <si>
@@ -555,7 +552,10 @@
     <t>CHARGING_TIME_STORAGE</t>
   </si>
   <si>
-    <t>5 hours</t>
+    <t>10 hours</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
@@ -1189,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC1002"/>
+  <dimension ref="A1:AC1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C100" workbookViewId="0">
-      <selection activeCell="W144" sqref="W144"/>
+    <sheetView tabSelected="1" topLeftCell="D106" workbookViewId="0">
+      <selection activeCell="D138" sqref="A138:XFD138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="109" spans="1:29" ht="14.25" customHeight="1">
       <c r="A109" s="52" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B109" s="15">
         <v>0.9</v>
@@ -5357,7 +5357,7 @@
     </row>
     <row r="110" spans="1:29" ht="14.25" customHeight="1">
       <c r="A110" s="52" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B110" s="32">
         <f>1.01^(1/HOURS_PER_YEAR)-1</f>
@@ -5400,7 +5400,7 @@
     </row>
     <row r="111" spans="1:29" ht="14.25" customHeight="1">
       <c r="A111" s="52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B111" s="40">
         <f>1568/261</f>
@@ -5755,7 +5755,7 @@
     </row>
     <row r="118" spans="1:29" ht="14.25" customHeight="1">
       <c r="A118" s="52" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B118" s="48">
         <f>1.0001^(1/HOURS_PER_YEAR)-1</f>
@@ -5798,7 +5798,7 @@
     </row>
     <row r="119" spans="1:29" ht="14.25" customHeight="1">
       <c r="A119" s="52" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B119" s="48">
         <v>0.3</v>
@@ -5867,7 +5867,7 @@
     </row>
     <row r="121" spans="1:29" s="53" customFormat="1">
       <c r="A121" s="52" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B121" s="59" t="s">
         <v>95</v>
@@ -5890,7 +5890,7 @@
         <v>2.7397260273972604E-6</v>
       </c>
       <c r="E122" s="58" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="123" spans="1:29" s="53" customFormat="1">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="D123" s="58"/>
       <c r="E123" s="58" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:29" s="53" customFormat="1">
@@ -5937,21 +5937,21 @@
     </row>
     <row r="126" spans="1:29" s="53" customFormat="1">
       <c r="A126" s="52" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B126" s="59">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="C126" s="58" t="s">
         <v>138</v>
       </c>
       <c r="E126" s="53" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:29" s="53" customFormat="1" ht="30">
       <c r="A127" s="52" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B127" s="59">
         <v>0.6</v>
@@ -6166,48 +6166,54 @@
         <v>116</v>
       </c>
       <c r="L134" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="M134" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="N134" s="52" t="s">
         <v>125</v>
       </c>
-      <c r="M134" s="52" t="s">
+      <c r="O134" s="52" t="s">
         <v>128</v>
       </c>
-      <c r="N134" s="52" t="s">
+      <c r="P134" s="52" t="s">
         <v>132</v>
       </c>
-      <c r="O134" s="52" t="s">
+      <c r="Q134" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="P134" s="52" t="s">
+      <c r="R134" s="52" t="s">
         <v>136</v>
       </c>
-      <c r="Q134" s="52" t="s">
+      <c r="S134" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="R134" s="52" t="s">
+      <c r="T134" s="52" t="s">
         <v>145</v>
       </c>
-      <c r="S134" s="52" t="s">
+      <c r="U134" s="52" t="s">
         <v>146</v>
       </c>
-      <c r="T134" s="52" t="s">
+      <c r="V134" s="52" t="s">
         <v>147</v>
       </c>
-      <c r="U134" s="52" t="s">
+      <c r="W134" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="V134" s="52" t="s">
+      <c r="X134" s="52" t="s">
         <v>157</v>
       </c>
-      <c r="W134" s="52" t="s">
+      <c r="Y134" s="52" t="s">
         <v>158</v>
       </c>
-      <c r="X134" s="52" t="s">
+      <c r="Z134" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="Y134" s="52" t="s">
+      <c r="AA134" s="52" t="s">
         <v>160</v>
       </c>
-      <c r="Z134" s="52" t="s">
+      <c r="AB134" s="52" t="s">
         <v>150</v>
       </c>
     </row>
@@ -6247,25 +6253,25 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="L136" s="54">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M136" s="54">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N136" s="54">
         <v>0.86666666666666003</v>
       </c>
-      <c r="M136" s="54">
+      <c r="O136" s="54">
         <v>0.86666666666666003</v>
-      </c>
-      <c r="N136" s="54">
-        <v>0.4</v>
-      </c>
-      <c r="O136" s="54">
-        <v>0.4</v>
       </c>
       <c r="P136" s="54">
         <v>0.4</v>
       </c>
       <c r="Q136" s="54">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="R136" s="54">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="S136" s="54">
         <v>0.2</v>
@@ -6277,10 +6283,10 @@
         <v>0.2</v>
       </c>
       <c r="V136" s="54">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="W136" s="54">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="X136" s="54">
         <v>1</v>
@@ -6289,6 +6295,12 @@
         <v>1</v>
       </c>
       <c r="Z136" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="AA136" s="54">
+        <v>0.2</v>
+      </c>
+      <c r="AB136" s="54">
         <v>1</v>
       </c>
     </row>
@@ -6368,98 +6380,55 @@
       <c r="Y137" s="55">
         <v>1</v>
       </c>
-      <c r="Z137" s="55">
+      <c r="Z137" s="55" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA137" s="55">
         <v>1</v>
       </c>
-    </row>
-    <row r="138" spans="1:29" s="55" customFormat="1">
-      <c r="A138" s="55" t="s">
-        <v>162</v>
-      </c>
-      <c r="B138" s="55">
-        <v>2015</v>
-      </c>
-      <c r="C138" s="55">
+      <c r="AB137" s="55">
         <v>1</v>
       </c>
-      <c r="D138" s="55">
-        <v>2015</v>
-      </c>
-      <c r="E138" s="55">
-        <v>1</v>
-      </c>
-      <c r="F138" s="54">
-        <v>0.6</v>
-      </c>
-      <c r="G138" s="54">
-        <v>0.6</v>
-      </c>
-      <c r="H138" s="54">
-        <v>1</v>
-      </c>
-      <c r="I138" s="54">
-        <v>1</v>
-      </c>
-      <c r="J138" s="54">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="K138" s="54">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="L138" s="54">
-        <v>0.86666666666666003</v>
-      </c>
-      <c r="M138" s="54">
-        <v>0.86666666666666003</v>
-      </c>
-      <c r="N138" s="54">
-        <v>0.4</v>
-      </c>
-      <c r="O138" s="54">
-        <v>0.4</v>
-      </c>
-      <c r="P138" s="54">
-        <v>0.4</v>
-      </c>
-      <c r="Q138" s="54">
-        <v>0.2</v>
-      </c>
-      <c r="R138" s="54">
-        <v>0.2</v>
-      </c>
-      <c r="S138" s="54">
-        <v>0.2</v>
-      </c>
-      <c r="T138" s="54">
-        <v>0.2</v>
-      </c>
-      <c r="U138" s="54">
-        <v>0.2</v>
-      </c>
-      <c r="V138" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="W138" s="55">
-        <v>0.3</v>
-      </c>
-      <c r="X138" s="55">
-        <v>1</v>
-      </c>
-      <c r="Y138" s="55">
-        <v>1</v>
-      </c>
-      <c r="Z138" s="55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139" spans="1:29" s="53" customFormat="1">
-      <c r="B139" s="56"/>
-    </row>
-    <row r="140" spans="1:29" s="49" customFormat="1">
-      <c r="A140" s="49" t="s">
+    </row>
+    <row r="138" spans="1:29" s="53" customFormat="1">
+      <c r="B138" s="56"/>
+    </row>
+    <row r="139" spans="1:29" s="49" customFormat="1">
+      <c r="A139" s="49" t="s">
         <v>156</v>
       </c>
-      <c r="B140" s="50"/>
+      <c r="B139" s="50"/>
+    </row>
+    <row r="140" spans="1:29" ht="14.25" customHeight="1">
+      <c r="A140" s="3"/>
+      <c r="B140" s="4"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="4"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="4"/>
+      <c r="G140" s="3"/>
+      <c r="H140" s="4"/>
+      <c r="I140" s="4"/>
+      <c r="J140" s="4"/>
+      <c r="K140" s="4"/>
+      <c r="L140" s="4"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="4"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="4"/>
+      <c r="Q140" s="4"/>
+      <c r="R140" s="4"/>
+      <c r="S140" s="4"/>
+      <c r="T140" s="4"/>
+      <c r="U140" s="4"/>
+      <c r="V140" s="4"/>
+      <c r="W140" s="4"/>
+      <c r="X140" s="4"/>
+      <c r="Y140" s="4"/>
+      <c r="Z140" s="4"/>
+      <c r="AA140" s="4"/>
+      <c r="AB140" s="4"/>
+      <c r="AC140" s="4"/>
     </row>
     <row r="141" spans="1:29" ht="14.25" customHeight="1">
       <c r="A141" s="3"/>
@@ -33152,37 +33121,6 @@
       <c r="AB1001" s="4"/>
       <c r="AC1001" s="4"/>
     </row>
-    <row r="1002" spans="1:29" ht="14.25" customHeight="1">
-      <c r="A1002" s="3"/>
-      <c r="B1002" s="4"/>
-      <c r="C1002" s="3"/>
-      <c r="D1002" s="4"/>
-      <c r="E1002" s="3"/>
-      <c r="F1002" s="4"/>
-      <c r="G1002" s="3"/>
-      <c r="H1002" s="4"/>
-      <c r="I1002" s="4"/>
-      <c r="J1002" s="4"/>
-      <c r="K1002" s="4"/>
-      <c r="L1002" s="4"/>
-      <c r="M1002" s="4"/>
-      <c r="N1002" s="4"/>
-      <c r="O1002" s="4"/>
-      <c r="P1002" s="4"/>
-      <c r="Q1002" s="4"/>
-      <c r="R1002" s="4"/>
-      <c r="S1002" s="4"/>
-      <c r="T1002" s="4"/>
-      <c r="U1002" s="4"/>
-      <c r="V1002" s="4"/>
-      <c r="W1002" s="4"/>
-      <c r="X1002" s="4"/>
-      <c r="Y1002" s="4"/>
-      <c r="Z1002" s="4"/>
-      <c r="AA1002" s="4"/>
-      <c r="AB1002" s="4"/>
-      <c r="AC1002" s="4"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C47" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>